<commit_message>
new modules for business logic and files
</commit_message>
<xml_diff>
--- a/data/posted invoices.xlsx
+++ b/data/posted invoices.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>reference</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>GF546</t>
+  </si>
+  <si>
+    <t>doc. number</t>
+  </si>
+  <si>
+    <t>vendor</t>
   </si>
 </sst>
 </file>
@@ -365,126 +371,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>12345</v>
+      </c>
+      <c r="B2">
+        <v>740000001</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="D2" s="1">
         <v>44280</v>
       </c>
-      <c r="C2" s="2">
+      <c r="E2" s="2">
         <v>2000.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>32564</v>
+      </c>
+      <c r="B3">
+        <v>740000002</v>
+      </c>
+      <c r="C3">
         <v>4568456315</v>
       </c>
-      <c r="B3" s="1">
+      <c r="D3" s="1">
         <v>43966</v>
       </c>
-      <c r="C3" s="2">
+      <c r="E3" s="2">
         <v>25102.35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>549879</v>
+      </c>
+      <c r="B4">
+        <v>740000003</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="D4" s="1">
         <v>44327</v>
       </c>
-      <c r="C4" s="2">
+      <c r="E4" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>45555</v>
+      </c>
+      <c r="B5">
+        <v>740000004</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="D5" s="1">
         <v>44280</v>
       </c>
-      <c r="C5" s="2">
+      <c r="E5" s="2">
         <v>2000.2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>489</v>
+      </c>
+      <c r="B6">
+        <v>740000005</v>
+      </c>
+      <c r="C6">
         <v>4567892</v>
       </c>
-      <c r="B6" s="1">
+      <c r="D6" s="1">
         <v>44275</v>
       </c>
-      <c r="C6" s="2">
+      <c r="E6" s="2">
         <v>1120.3599999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>32654</v>
+      </c>
+      <c r="B7">
+        <v>740000006</v>
+      </c>
+      <c r="C7">
         <v>16548</v>
       </c>
-      <c r="B7" s="1">
+      <c r="D7" s="1">
         <v>44058</v>
       </c>
-      <c r="C7" s="2">
+      <c r="E7" s="2">
         <v>45851.12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>587646</v>
+      </c>
+      <c r="B8">
+        <v>740000007</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1">
+      <c r="D8" s="1">
         <v>44219</v>
       </c>
-      <c r="C8" s="2">
+      <c r="E8" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>687465</v>
+      </c>
+      <c r="B9">
+        <v>740000008</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="1">
+      <c r="D9" s="1">
         <v>44296</v>
       </c>
-      <c r="C9" s="2">
+      <c r="E9" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>66846</v>
+      </c>
+      <c r="B10">
+        <v>740000009</v>
+      </c>
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
+      <c r="D10" s="1">
         <v>44327</v>
       </c>
-      <c r="C10" s="2">
+      <c r="E10" s="2">
         <v>105</v>
       </c>
     </row>

</xml_diff>